<commit_message>
Updated column format as number for unique id
</commit_message>
<xml_diff>
--- a/import-instagram-data-template.xlsx
+++ b/import-instagram-data-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\inhouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816ABCC1-A528-454D-BAC4-20B57E33924A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB6DD2E-40F9-499C-8243-B6D275614363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{41DC7B45-5F82-4C05-8E1C-3373362029E4}"/>
   </bookViews>
@@ -179,13 +179,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,12 +504,12 @@
   <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -545,7 +546,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">

</xml_diff>